<commit_message>
Arrumando classe vendas para CRUDVendas
</commit_message>
<xml_diff>
--- a/download_relatorio/relatorio_vendas.xlsx
+++ b/download_relatorio/relatorio_vendas.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,7 +471,7 @@
   <cols>
     <col width="4" customWidth="1" min="1" max="1"/>
     <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="24" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
     <col width="7" customWidth="1" min="5" max="5"/>
     <col width="21" customWidth="1" min="6" max="6"/>
@@ -511,7 +511,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B2" s="4" t="inlineStr">
         <is>
@@ -520,26 +520,26 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>sa</t>
+          <t>Aline de Lucas</t>
         </is>
       </c>
       <c r="D2" s="4" t="inlineStr">
         <is>
-          <t>dinheiro</t>
+          <t>cartao</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
         <is>
-          <t>2.50</t>
+          <t>5.00</t>
         </is>
       </c>
       <c r="F2" s="5" t="n">
-        <v>45630.96983796296</v>
+        <v>45634.89003472222</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
@@ -554,16 +554,16 @@
       </c>
       <c r="E3" s="4" t="inlineStr">
         <is>
-          <t>5.00</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="F3" s="5" t="n">
-        <v>45633.74258101852</v>
+        <v>45634.89733796296</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
@@ -571,23 +571,19 @@
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr"/>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>dinheiro</t>
-        </is>
-      </c>
+      <c r="D4" s="4" t="inlineStr"/>
       <c r="E4" s="4" t="inlineStr">
         <is>
-          <t>5.00</t>
+          <t>10.29</t>
         </is>
       </c>
       <c r="F4" s="5" t="n">
-        <v>45633.75076388889</v>
+        <v>45634.90263888889</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
@@ -596,26 +592,22 @@
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
-          <t>sa</t>
-        </is>
-      </c>
-      <c r="D5" s="4" t="inlineStr">
-        <is>
-          <t>dinheiro</t>
-        </is>
-      </c>
+          <t>Aline de Lucas</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="inlineStr"/>
       <c r="E5" s="4" t="inlineStr">
         <is>
           <t>5.00</t>
         </is>
       </c>
       <c r="F5" s="5" t="n">
-        <v>45633.75555555556</v>
+        <v>45634.90609953704</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
@@ -624,26 +616,26 @@
       </c>
       <c r="C6" s="4" t="inlineStr">
         <is>
-          <t>Murilo Dantas</t>
+          <t>Murilo da Silva Dantas</t>
         </is>
       </c>
       <c r="D6" s="4" t="inlineStr">
         <is>
-          <t>dinheiro</t>
+          <t>pix</t>
         </is>
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
-          <t>5.00</t>
+          <t>35.46</t>
         </is>
       </c>
       <c r="F6" s="5" t="n">
-        <v>45633.77445601852</v>
+        <v>45634.91111111111</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
@@ -662,12 +654,12 @@
         </is>
       </c>
       <c r="F7" s="5" t="n">
-        <v>45633.77560185185</v>
+        <v>45634.91421296296</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="n">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B8" s="4" t="inlineStr">
         <is>
@@ -676,7 +668,7 @@
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t>Pedro de Moraes</t>
+          <t>Murilo da Silva Dantas</t>
         </is>
       </c>
       <c r="D8" s="4" t="inlineStr">
@@ -686,331 +678,11 @@
       </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t>2.00</t>
+          <t>31.74</t>
         </is>
       </c>
       <c r="F8" s="5" t="n">
-        <v>45633.83293981481</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="n">
-        <v>14</v>
-      </c>
-      <c r="B9" s="4" t="inlineStr">
-        <is>
-          <t>aluno</t>
-        </is>
-      </c>
-      <c r="C9" s="4" t="inlineStr"/>
-      <c r="D9" s="4" t="inlineStr">
-        <is>
-          <t>dinheiro</t>
-        </is>
-      </c>
-      <c r="E9" s="4" t="inlineStr">
-        <is>
-          <t>1.00</t>
-        </is>
-      </c>
-      <c r="F9" s="5" t="n">
-        <v>45633.83332175926</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="n">
-        <v>15</v>
-      </c>
-      <c r="B10" s="4" t="inlineStr">
-        <is>
-          <t>funcionario</t>
-        </is>
-      </c>
-      <c r="C10" s="4" t="inlineStr">
-        <is>
-          <t>sa</t>
-        </is>
-      </c>
-      <c r="D10" s="4" t="inlineStr">
-        <is>
-          <t>dinheiro</t>
-        </is>
-      </c>
-      <c r="E10" s="4" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="F10" s="5" t="n">
-        <v>45633.84258101852</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="n">
-        <v>16</v>
-      </c>
-      <c r="B11" s="4" t="inlineStr">
-        <is>
-          <t>funcionario</t>
-        </is>
-      </c>
-      <c r="C11" s="4" t="inlineStr">
-        <is>
-          <t>Pedro de Moraes</t>
-        </is>
-      </c>
-      <c r="D11" s="4" t="inlineStr">
-        <is>
-          <t>dinheiro</t>
-        </is>
-      </c>
-      <c r="E11" s="4" t="inlineStr">
-        <is>
-          <t>2.50</t>
-        </is>
-      </c>
-      <c r="F11" s="5" t="n">
-        <v>45633.86983796296</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="n">
-        <v>17</v>
-      </c>
-      <c r="B12" s="4" t="inlineStr">
-        <is>
-          <t>aluno</t>
-        </is>
-      </c>
-      <c r="C12" s="4" t="inlineStr"/>
-      <c r="D12" s="4" t="inlineStr">
-        <is>
-          <t>dinheiro</t>
-        </is>
-      </c>
-      <c r="E12" s="4" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="F12" s="5" t="n">
-        <v>45634.11862268519</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="n">
-        <v>18</v>
-      </c>
-      <c r="B13" s="4" t="inlineStr">
-        <is>
-          <t>funcionario</t>
-        </is>
-      </c>
-      <c r="C13" s="4" t="inlineStr">
-        <is>
-          <t>Pedro de Moraes</t>
-        </is>
-      </c>
-      <c r="D13" s="4" t="inlineStr">
-        <is>
-          <t>dinheiro</t>
-        </is>
-      </c>
-      <c r="E13" s="4" t="inlineStr">
-        <is>
-          <t>5.00</t>
-        </is>
-      </c>
-      <c r="F13" s="5" t="n">
-        <v>45634.59497685185</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="n">
-        <v>19</v>
-      </c>
-      <c r="B14" s="4" t="inlineStr">
-        <is>
-          <t>funcionario</t>
-        </is>
-      </c>
-      <c r="C14" s="4" t="inlineStr">
-        <is>
-          <t>Murilo Dantas</t>
-        </is>
-      </c>
-      <c r="D14" s="4" t="inlineStr">
-        <is>
-          <t>dinheiro</t>
-        </is>
-      </c>
-      <c r="E14" s="4" t="inlineStr">
-        <is>
-          <t>2.50</t>
-        </is>
-      </c>
-      <c r="F14" s="5" t="n">
-        <v>45634.60317129629</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="B15" s="4" t="inlineStr">
-        <is>
-          <t>funcionario</t>
-        </is>
-      </c>
-      <c r="C15" s="4" t="inlineStr">
-        <is>
-          <t>Murilo Dantas</t>
-        </is>
-      </c>
-      <c r="D15" s="4" t="inlineStr">
-        <is>
-          <t>dinheiro</t>
-        </is>
-      </c>
-      <c r="E15" s="4" t="inlineStr">
-        <is>
-          <t>18.00</t>
-        </is>
-      </c>
-      <c r="F15" s="5" t="n">
-        <v>45634.60600694444</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="n">
-        <v>21</v>
-      </c>
-      <c r="B16" s="4" t="inlineStr">
-        <is>
-          <t>funcionario</t>
-        </is>
-      </c>
-      <c r="C16" s="4" t="inlineStr">
-        <is>
-          <t>Murilo Dantas</t>
-        </is>
-      </c>
-      <c r="D16" s="4" t="inlineStr">
-        <is>
-          <t>dinheiro</t>
-        </is>
-      </c>
-      <c r="E16" s="4" t="inlineStr">
-        <is>
-          <t>5.50</t>
-        </is>
-      </c>
-      <c r="F16" s="5" t="n">
-        <v>45634.63700231481</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="n">
-        <v>22</v>
-      </c>
-      <c r="B17" s="4" t="inlineStr">
-        <is>
-          <t>aluno</t>
-        </is>
-      </c>
-      <c r="C17" s="4" t="inlineStr"/>
-      <c r="D17" s="4" t="inlineStr">
-        <is>
-          <t>dinheiro</t>
-        </is>
-      </c>
-      <c r="E17" s="4" t="inlineStr">
-        <is>
-          <t>2.50</t>
-        </is>
-      </c>
-      <c r="F17" s="5" t="n">
-        <v>45634.64412037037</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="n">
-        <v>23</v>
-      </c>
-      <c r="B18" s="4" t="inlineStr">
-        <is>
-          <t>funcionario</t>
-        </is>
-      </c>
-      <c r="C18" s="4" t="inlineStr">
-        <is>
-          <t>sa</t>
-        </is>
-      </c>
-      <c r="D18" s="4" t="inlineStr">
-        <is>
-          <t>dinheiro</t>
-        </is>
-      </c>
-      <c r="E18" s="4" t="inlineStr">
-        <is>
-          <t>2.50</t>
-        </is>
-      </c>
-      <c r="F18" s="5" t="n">
-        <v>45634.65527777778</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="4" t="n">
-        <v>24</v>
-      </c>
-      <c r="B19" s="4" t="inlineStr">
-        <is>
-          <t>aluno</t>
-        </is>
-      </c>
-      <c r="C19" s="4" t="inlineStr"/>
-      <c r="D19" s="4" t="inlineStr">
-        <is>
-          <t>dinheiro</t>
-        </is>
-      </c>
-      <c r="E19" s="4" t="inlineStr">
-        <is>
-          <t>11.00</t>
-        </is>
-      </c>
-      <c r="F19" s="5" t="n">
-        <v>45634.70886574074</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="n">
-        <v>25</v>
-      </c>
-      <c r="B20" s="4" t="inlineStr">
-        <is>
-          <t>funcionario</t>
-        </is>
-      </c>
-      <c r="C20" s="4" t="inlineStr">
-        <is>
-          <t>Murilo Dantas</t>
-        </is>
-      </c>
-      <c r="D20" s="4" t="inlineStr">
-        <is>
-          <t>dinheiro</t>
-        </is>
-      </c>
-      <c r="E20" s="4" t="inlineStr">
-        <is>
-          <t>5.50</t>
-        </is>
-      </c>
-      <c r="F20" s="5" t="n">
-        <v>45634.70912037037</v>
+        <v>45635.01660879629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>